<commit_message>
Rename key inputs and include some portfolio optimization upates
</commit_message>
<xml_diff>
--- a/paola/PortfolioRecommendation.xlsx
+++ b/paola/PortfolioRecommendation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paola/FinTech/Projects/awesome_retirement_portfolio_projector_tool/paola/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1BEF53-7F9B-1F4B-8208-D2A95422DDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60879910-DCF8-8D49-90CB-E8784C8F13BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{E26525CA-416E-8C42-B628-E3219ADAECD7}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
-    <t>Current position</t>
-  </si>
-  <si>
     <t>APPL</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Other %</t>
   </si>
   <si>
-    <t>Additional Instruments for recommendation</t>
-  </si>
-  <si>
     <t>SPY</t>
   </si>
   <si>
@@ -133,6 +127,12 @@
   </si>
   <si>
     <t>3 - EQUITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Portfolio </t>
+  </si>
+  <si>
+    <t>Additional Instruments for diversification in recommendation</t>
   </si>
 </sst>
 </file>
@@ -601,15 +601,6 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="3" applyBorder="1"/>
@@ -629,6 +620,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1094,36 +1094,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="G1" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="26" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1132,102 +1132,102 @@
         <v>11612.619999999999</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="2">
         <v>5</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="24">
         <v>145.79</v>
       </c>
-      <c r="G3" s="34">
+      <c r="G3" s="31">
         <v>1</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="32">
         <v>0</v>
       </c>
-      <c r="I3" s="36">
+      <c r="I3" s="33">
         <v>0</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="27">
         <f>(E3*F3)/$A$3</f>
         <v>6.2772225389274766E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D4" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2">
         <v>20</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="24">
         <v>86.16</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G4" s="31">
         <v>1</v>
       </c>
-      <c r="H4" s="35">
+      <c r="H4" s="32">
         <v>0</v>
       </c>
-      <c r="I4" s="36">
+      <c r="I4" s="33">
         <v>0</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="27">
         <f t="shared" ref="J4:J6" si="0">(E4*F4)/$A$3</f>
         <v>0.14839028574085777</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="24">
         <v>2757.77</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
-      <c r="H5" s="35">
+      <c r="H5" s="32">
         <v>0</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="33">
         <v>0</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="27">
         <f t="shared" si="0"/>
         <v>0.71244129231818487</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="25">
         <v>443.58</v>
       </c>
-      <c r="G6" s="37">
+      <c r="G6" s="34">
         <v>1</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="35">
         <v>0</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="36">
         <v>0</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="28">
         <f t="shared" si="0"/>
         <v>7.6396196551682574E-2</v>
       </c>
@@ -1250,7 +1250,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D9" s="11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1260,7 +1260,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D11" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1292,87 +1292,87 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D12" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="E16" s="41" t="s">
-        <v>29</v>
+      <c r="E16" s="38" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F21" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>30</v>
+      <c r="F22" s="40" t="s">
+        <v>28</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J22" s="40"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="37"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J23" s="40"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="37"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>32</v>
+        <v>16</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>30</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="40"/>
+        <v>2</v>
+      </c>
+      <c r="J24" s="37"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J25" s="40"/>
+        <v>6</v>
+      </c>
+      <c r="J25" s="37"/>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="40"/>
+        <v>7</v>
+      </c>
+      <c r="J26" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
upload optimization function working
</commit_message>
<xml_diff>
--- a/paola/PortfolioRecommendation.xlsx
+++ b/paola/PortfolioRecommendation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paola/FinTech/Projects/awesome_retirement_portfolio_projector_tool/paola/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60879910-DCF8-8D49-90CB-E8784C8F13BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C79A97-60BD-FC40-9669-A3F34BD0C834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{E26525CA-416E-8C42-B628-E3219ADAECD7}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>APPL</t>
   </si>
   <si>
-    <t>XLB</t>
-  </si>
-  <si>
-    <t>GOOG</t>
-  </si>
-  <si>
     <t>Equity %</t>
   </si>
   <si>
@@ -87,24 +81,12 @@
     <t>10-20%</t>
   </si>
   <si>
-    <t>Portfolio to optimize</t>
-  </si>
-  <si>
-    <t>Optimized allocation</t>
-  </si>
-  <si>
     <t>The additional instruments, extendable to more variety of markets: International, Fixed Income (Corporate&amp;Soberan distinction, Duration distinction)</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Current allocation</t>
-  </si>
-  <si>
     <t>Current portfolio value</t>
   </si>
   <si>
@@ -133,6 +115,33 @@
   </si>
   <si>
     <t>Additional Instruments for diversification in recommendation</t>
+  </si>
+  <si>
+    <t>CSCO</t>
+  </si>
+  <si>
+    <t>Original weights</t>
+  </si>
+  <si>
+    <t>OUTPUT FROM OPTIMIZATION</t>
+  </si>
+  <si>
+    <t>INPUT TO OPTIMIZATION AND VISUALIZATION</t>
+  </si>
+  <si>
+    <t>INPUT FOR VISUALIZATION</t>
+  </si>
+  <si>
+    <t>Current Price</t>
+  </si>
+  <si>
+    <t>OUTPUT FROM FRONT END &amp; API CALLS</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Optimized weights</t>
   </si>
 </sst>
 </file>
@@ -217,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -564,6 +573,21 @@
         <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -575,7 +599,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -593,14 +617,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="3" applyBorder="1"/>
@@ -615,7 +637,6 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="24" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="25" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -629,6 +650,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -655,13 +684,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2597150</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -715,13 +744,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>406399</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>63499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>130174</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -738,6 +767,66 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7912099" y="3759199"/>
+          <a:ext cx="854075" cy="1184275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Right Arrow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57409E07-1C34-8A4D-A1F9-C1CF9FF74CE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12890500" y="76200"/>
           <a:ext cx="854075" cy="1184275"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
@@ -1071,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16612C2B-E9C5-1445-ADB6-5D3EC6CF1884}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1171,7 @@
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" customWidth="1"/>
     <col min="8" max="8" width="13.1640625" customWidth="1"/>
     <col min="9" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -1093,290 +1182,325 @@
     <col min="15" max="15" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="43"/>
+      <c r="M3" s="44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="20">
+        <f>SUMPRODUCT(E4:E7,F4:F7)</f>
+        <v>2735.7099999999996</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="22">
+        <v>145.79</v>
+      </c>
+      <c r="G4" s="29">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30">
+        <v>0</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="25">
+        <f>(E4*F4)/$A$4</f>
+        <v>0.26645733648668901</v>
+      </c>
+      <c r="L4" s="6" t="str">
+        <f>D4</f>
+        <v>APPL</v>
+      </c>
+      <c r="M4" s="45">
+        <f>J4</f>
+        <v>0.26645733648668901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2">
         <v>20</v>
       </c>
-      <c r="F2" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="30" t="s">
+      <c r="F5" s="22">
+        <v>55.98</v>
+      </c>
+      <c r="G5" s="29">
+        <v>1</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25">
+        <f t="shared" ref="J5:L7" si="0">(E5*F5)/$A$4</f>
+        <v>0.40925390483640445</v>
+      </c>
+      <c r="L5" s="6" t="str">
+        <f>D5</f>
+        <v>CSCO</v>
+      </c>
+      <c r="M5" s="45">
+        <f>J5</f>
+        <v>0.40925390483640445</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>4</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="21">
-        <f>SUMPRODUCT(E3:E6,F3:F6)</f>
-        <v>11612.619999999999</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>5</v>
-      </c>
-      <c r="F3" s="24">
-        <v>145.79</v>
-      </c>
-      <c r="G3" s="31">
-        <v>1</v>
-      </c>
-      <c r="H3" s="32">
-        <v>0</v>
-      </c>
-      <c r="I3" s="33">
-        <v>0</v>
-      </c>
-      <c r="J3" s="27">
-        <f>(E3*F3)/$A$3</f>
-        <v>6.2772225389274766E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>20</v>
-      </c>
-      <c r="F4" s="24">
-        <v>86.16</v>
-      </c>
-      <c r="G4" s="31">
-        <v>1</v>
-      </c>
-      <c r="H4" s="32">
-        <v>0</v>
-      </c>
-      <c r="I4" s="33">
-        <v>0</v>
-      </c>
-      <c r="J4" s="27">
-        <f t="shared" ref="J4:J6" si="0">(E4*F4)/$A$3</f>
-        <v>0.14839028574085777</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="24">
-        <v>2757.77</v>
-      </c>
-      <c r="G5" s="31">
-        <v>1</v>
-      </c>
-      <c r="H5" s="32">
-        <v>0</v>
-      </c>
-      <c r="I5" s="33">
-        <v>0</v>
-      </c>
-      <c r="J5" s="27">
-        <f t="shared" si="0"/>
-        <v>0.71244129231818487</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>6</v>
       </c>
       <c r="E6" s="13">
         <v>2</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="23">
         <v>443.58</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="32">
         <v>1</v>
       </c>
-      <c r="H6" s="35">
+      <c r="H6" s="33">
         <v>0</v>
       </c>
-      <c r="I6" s="36">
+      <c r="I6" s="34">
         <v>0</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="26">
         <f t="shared" si="0"/>
-        <v>7.6396196551682574E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.3242887586769066</v>
+      </c>
+      <c r="L6" s="6" t="str">
+        <f>D6</f>
+        <v>SPY</v>
+      </c>
+      <c r="M6" s="45">
+        <f>J6</f>
+        <v>0.3242887586769066</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="L7" s="12" t="str">
+        <f>D11</f>
+        <v>AGG</v>
+      </c>
+      <c r="M7" s="46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D9" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D10" s="6" t="s">
-        <v>6</v>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D10" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="3">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I11" s="15">
         <v>0</v>
       </c>
-      <c r="I10" s="15">
+    </row>
+    <row r="12" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14">
+      <c r="I12" s="16">
         <v>0</v>
       </c>
-      <c r="H11" s="14">
-        <v>1</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="26" x14ac:dyDescent="0.3">
-      <c r="E16" s="38" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="20" t="s">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D13" s="42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" ht="26" x14ac:dyDescent="0.3">
+      <c r="E17" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="E22" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="40" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="37"/>
-    </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="37"/>
+      <c r="F23" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f>D4</f>
+        <v>APPL</v>
+      </c>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J24" s="37"/>
+        <v>13</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <f>D5</f>
+        <v>CSCO</v>
+      </c>
+      <c r="J24" s="48"/>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="I25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="37"/>
-    </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="I26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="37"/>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f>D6</f>
+        <v>SPY</v>
+      </c>
+      <c r="J25" s="48"/>
+    </row>
+    <row r="26" spans="4:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="12" t="str">
+        <f>D11</f>
+        <v>AGG</v>
+      </c>
+      <c r="J26" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>